<commit_message>
new variable Aridity created for models
</commit_message>
<xml_diff>
--- a/AbuPhyl.xlsx
+++ b/AbuPhyl.xlsx
@@ -5416,7 +5416,7 @@
         </is>
       </c>
       <c r="BO16">
-        <v>7.650825749915739</v>
+        <v>7.65082574991574</v>
       </c>
     </row>
     <row r="17">
@@ -27466,7 +27466,7 @@
         </is>
       </c>
       <c r="BO86">
-        <v>23.21789686552072</v>
+        <v>23.21789686552073</v>
       </c>
     </row>
     <row r="87">
@@ -28411,7 +28411,7 @@
         </is>
       </c>
       <c r="BO89">
-        <v>18.62487360970677</v>
+        <v>18.62487360970678</v>
       </c>
     </row>
     <row r="90">

</xml_diff>